<commit_message>
7:19 am Jan 28 2012
</commit_message>
<xml_diff>
--- a/PlayingFieldData.xlsx
+++ b/PlayingFieldData.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="100" windowWidth="12000" windowHeight="13180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,11 +12,16 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="58">
   <si>
     <t>true</t>
   </si>
@@ -175,22 +180,50 @@
   </si>
   <si>
     <t>[48,     39]</t>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Verdana"/>
     </font>
   </fonts>
   <fills count="2">
@@ -223,7 +256,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -511,23 +544,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:O63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="5" max="5" width="8" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.6640625" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="18.5703125" customWidth="1"/>
-    <col min="11" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="13.28515625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="18.5" customWidth="1"/>
+    <col min="11" max="14" width="16.6640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" s="2" customFormat="1">
@@ -593,13 +626,13 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>3</v>
@@ -609,7 +642,7 @@
       </c>
       <c r="K2" s="2" t="str">
         <f>CONCATENATE($A$1, A2, $B$1, B2, $C$1, C2, $D$1, D2, $E$1, E2, $F$1, F2, $G$1, G2, $H$1, H2, $I$1, I2, $J$1, J2, $K$1)</f>
-        <v>{ X: 0, Y:0, Width: 0.05, Height: 0.1, Label: 0, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [1, 10], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0, Y:0, Width: 0.05, Height: 0.1, Label: 0, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [1, 10], CostalRestrictions: [[]] }</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -632,13 +665,13 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>4</v>
@@ -648,7 +681,7 @@
       </c>
       <c r="K3" s="2" t="str">
         <f t="shared" ref="K3:K51" si="0">CONCATENATE($A$1, A3, $B$1, B3, $C$1, C3, $D$1, D3, $E$1, E3, $F$1, F3, $G$1, G3, $H$1, H3, $I$1, I3, $J$1, J3, $K$1)</f>
-        <v>{ X: 0.1, Y:0, Width: 0.05, Height: 0.1, Label: 1, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [0, 2, 11], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.1, Y:0, Width: 0.05, Height: 0.1, Label: 1, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [0, 2, 11], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -668,13 +701,13 @@
         <v>2</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I4" s="1" t="s">
         <v>5</v>
@@ -684,7 +717,7 @@
       </c>
       <c r="K4" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.2, Y:0, Width: 0.05, Height: 0.1, Label: 2, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [1, 3, 12], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.2, Y:0, Width: 0.05, Height: 0.1, Label: 2, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: true, Connections: [1, 3, 12], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -707,10 +740,10 @@
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I5" s="1" t="s">
         <v>6</v>
@@ -720,7 +753,7 @@
       </c>
       <c r="K5" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.3, Y:0, Width: 0.05, Height: 0.1, Label: 3, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [2, 4, 13], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.3, Y:0, Width: 0.05, Height: 0.1, Label: 3, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [2, 4, 13], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -743,10 +776,10 @@
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I6" s="1" t="s">
         <v>7</v>
@@ -756,7 +789,7 @@
       </c>
       <c r="K6" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.4, Y:0, Width: 0.05, Height: 0.1, Label: 4, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [3, 5, 14], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.4, Y:0, Width: 0.05, Height: 0.1, Label: 4, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [3, 5, 14], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -779,10 +812,10 @@
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I7" s="1" t="s">
         <v>8</v>
@@ -792,7 +825,7 @@
       </c>
       <c r="K7" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.5, Y:0, Width: 0.05, Height: 0.1, Label: 5, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [4, 6, 15], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.5, Y:0, Width: 0.05, Height: 0.1, Label: 5, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [4, 6, 15], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -818,7 +851,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I8" s="1" t="s">
         <v>9</v>
@@ -828,7 +861,7 @@
       </c>
       <c r="K8" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.6, Y:0, Width: 0.05, Height: 0.1, Label: 6, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [5, 7, 16], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.6, Y:0, Width: 0.05, Height: 0.1, Label: 6, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [5, 7, 16], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -854,7 +887,7 @@
         <v>1</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>10</v>
@@ -890,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I10" s="1" t="s">
         <v>11</v>
@@ -900,7 +933,7 @@
       </c>
       <c r="K10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.8, Y:0, Width: 0.05, Height: 0.1, Label: 8, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [7, 9, 18], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.8, Y:0, Width: 0.05, Height: 0.1, Label: 8, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [7, 9, 18], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -926,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I11" s="1" t="s">
         <v>12</v>
@@ -959,10 +992,10 @@
         <v>0</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>13</v>
@@ -972,7 +1005,7 @@
       </c>
       <c r="K12" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0, Y:0.2, Width: 0.05, Height: 0.1, Label: 10, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [    11, 20, 0], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0, Y:0.2, Width: 0.05, Height: 0.1, Label: 10, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: true, Connections: [    11, 20, 0], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -992,13 +1025,13 @@
         <v>11</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>0</v>
+        <v>57</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>14</v>
@@ -1008,7 +1041,7 @@
       </c>
       <c r="K13" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.1, Y:0.2, Width: 0.05, Height: 0.1, Label: 11, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [10, 12, 21, 1], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.1, Y:0.2, Width: 0.05, Height: 0.1, Label: 11, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [10, 12, 21, 1], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -1028,13 +1061,13 @@
         <v>12</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>15</v>
@@ -1044,7 +1077,7 @@
       </c>
       <c r="K14" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.2, Y:0.2, Width: 0.05, Height: 0.1, Label: 12, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [11, 13, 22, 2], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.2, Y:0.2, Width: 0.05, Height: 0.1, Label: 12, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [11, 13, 22, 2], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -1067,10 +1100,10 @@
         <v>0</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>16</v>
@@ -1080,7 +1113,7 @@
       </c>
       <c r="K15" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.3, Y:0.2, Width: 0.05, Height: 0.1, Label: 13, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [12, 14, 23, 3], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.3, Y:0.2, Width: 0.05, Height: 0.1, Label: 13, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [12, 14, 23, 3], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -1103,10 +1136,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>17</v>
@@ -1116,7 +1149,7 @@
       </c>
       <c r="K16" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.4, Y:0.2, Width: 0.05, Height: 0.1, Label: 14, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [13, 15, 24, 4], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.4, Y:0.2, Width: 0.05, Height: 0.1, Label: 14, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [13, 15, 24, 4], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -1136,13 +1169,13 @@
         <v>15</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>18</v>
@@ -1152,7 +1185,7 @@
       </c>
       <c r="K17" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.5, Y:0.2, Width: 0.05, Height: 0.1, Label: 15, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [14, 16, 25, 5], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.5, Y:0.2, Width: 0.05, Height: 0.1, Label: 15, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [14, 16, 25, 5], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -1175,10 +1208,10 @@
         <v>0</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>19</v>
@@ -1188,7 +1221,7 @@
       </c>
       <c r="K18" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.6, Y:0.2, Width: 0.05, Height: 0.1, Label: 16, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [15, 17, 26, 6], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.6, Y:0.2, Width: 0.05, Height: 0.1, Label: 16, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [15, 17, 26, 6], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="19" spans="1:11">
@@ -1214,7 +1247,7 @@
         <v>1</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>20</v>
@@ -1224,7 +1257,7 @@
       </c>
       <c r="K19" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.7, Y:0.2, Width: 0.05, Height: 0.1, Label: 17, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [16, 18, 27, 7], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.7, Y:0.2, Width: 0.05, Height: 0.1, Label: 17, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [16, 18, 27, 7], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="20" spans="1:11">
@@ -1250,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>21</v>
@@ -1260,7 +1293,7 @@
       </c>
       <c r="K20" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.8, Y:0.2, Width: 0.05, Height: 0.1, Label: 18, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [17, 19, 28, 8], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.8, Y:0.2, Width: 0.05, Height: 0.1, Label: 18, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [17, 19, 28, 8], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="21" spans="1:11">
@@ -1286,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I21" s="1" t="s">
         <v>22</v>
@@ -1296,7 +1329,7 @@
       </c>
       <c r="K21" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.9, Y:0.2, Width: 0.05, Height: 0.1, Label: 19, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [18,     29, 9], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.9, Y:0.2, Width: 0.05, Height: 0.1, Label: 19, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [18,     29, 9], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="22" spans="1:11">
@@ -1319,10 +1352,10 @@
         <v>0</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>23</v>
@@ -1332,7 +1365,7 @@
       </c>
       <c r="K22" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0, Y:0.4, Width: 0.05, Height: 0.1, Label: 20, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [    21, 30, 10], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0, Y:0.4, Width: 0.05, Height: 0.1, Label: 20, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [    21, 30, 10], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="23" spans="1:11">
@@ -1352,13 +1385,13 @@
         <v>21</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>24</v>
@@ -1368,7 +1401,7 @@
       </c>
       <c r="K23" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.1, Y:0.4, Width: 0.05, Height: 0.1, Label: 21, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [20, 22, 31, 11], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.1, Y:0.4, Width: 0.05, Height: 0.1, Label: 21, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [20, 22, 31, 11], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="24" spans="1:11">
@@ -1388,13 +1421,13 @@
         <v>22</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>25</v>
@@ -1404,7 +1437,7 @@
       </c>
       <c r="K24" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.2, Y:0.4, Width: 0.05, Height: 0.1, Label: 22, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [21, 23, 32, 12], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.2, Y:0.4, Width: 0.05, Height: 0.1, Label: 22, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [21, 23, 32, 12], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="25" spans="1:11">
@@ -1427,10 +1460,10 @@
         <v>0</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I25" s="1" t="s">
         <v>26</v>
@@ -1440,7 +1473,7 @@
       </c>
       <c r="K25" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.3, Y:0.4, Width: 0.05, Height: 0.1, Label: 23, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [22, 24, 33, 13], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.3, Y:0.4, Width: 0.05, Height: 0.1, Label: 23, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [22, 24, 33, 13], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="26" spans="1:11">
@@ -1463,10 +1496,10 @@
         <v>0</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>27</v>
@@ -1476,7 +1509,7 @@
       </c>
       <c r="K26" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.4, Y:0.4, Width: 0.05, Height: 0.1, Label: 24, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [23, 25, 34, 14], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.4, Y:0.4, Width: 0.05, Height: 0.1, Label: 24, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [23, 25, 34, 14], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="27" spans="1:11">
@@ -1496,13 +1529,13 @@
         <v>25</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>28</v>
@@ -1512,7 +1545,7 @@
       </c>
       <c r="K27" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.5, Y:0.4, Width: 0.05, Height: 0.1, Label: 25, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [24, 26, 35, 15], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.5, Y:0.4, Width: 0.05, Height: 0.1, Label: 25, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: true, Connections: [24, 26, 35, 15], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="28" spans="1:11">
@@ -1532,13 +1565,13 @@
         <v>26</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I28" s="1" t="s">
         <v>29</v>
@@ -1548,7 +1581,7 @@
       </c>
       <c r="K28" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.6, Y:0.4, Width: 0.05, Height: 0.1, Label: 26, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [25, 27, 36, 16], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.6, Y:0.4, Width: 0.05, Height: 0.1, Label: 26, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [25, 27, 36, 16], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="29" spans="1:11">
@@ -1568,13 +1601,13 @@
         <v>27</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I29" s="1" t="s">
         <v>30</v>
@@ -1584,7 +1617,7 @@
       </c>
       <c r="K29" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.7, Y:0.4, Width: 0.05, Height: 0.1, Label: 27, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [26, 28, 37, 17], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.7, Y:0.4, Width: 0.05, Height: 0.1, Label: 27, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: true, Connections: [26, 28, 37, 17], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="30" spans="1:11">
@@ -1607,10 +1640,10 @@
         <v>0</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>1</v>
+        <v>55</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>31</v>
@@ -1620,7 +1653,7 @@
       </c>
       <c r="K30" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.8, Y:0.4, Width: 0.05, Height: 0.1, Label: 28, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [27, 29, 38, 18], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.8, Y:0.4, Width: 0.05, Height: 0.1, Label: 28, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: true, Connections: [27, 29, 38, 18], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="31" spans="1:11">
@@ -1643,10 +1676,10 @@
         <v>0</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I31" s="1" t="s">
         <v>32</v>
@@ -1679,10 +1712,10 @@
         <v>0</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>33</v>
@@ -1692,7 +1725,7 @@
       </c>
       <c r="K32" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0, Y:0.6, Width: 0.05, Height: 0.1, Label: 30, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [    31, 40, 20], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0, Y:0.6, Width: 0.05, Height: 0.1, Label: 30, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [    31, 40, 20], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="33" spans="1:11">
@@ -1715,10 +1748,10 @@
         <v>0</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>34</v>
@@ -1728,7 +1761,7 @@
       </c>
       <c r="K33" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.1, Y:0.6, Width: 0.05, Height: 0.1, Label: 31, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [30, 32, 41, 21], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.1, Y:0.6, Width: 0.05, Height: 0.1, Label: 31, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [30, 32, 41, 21], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="34" spans="1:11">
@@ -1751,10 +1784,10 @@
         <v>0</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>35</v>
@@ -1764,7 +1797,7 @@
       </c>
       <c r="K34" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.2, Y:0.6, Width: 0.05, Height: 0.1, Label: 32, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [31, 33, 42, 22], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.2, Y:0.6, Width: 0.05, Height: 0.1, Label: 32, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [31, 33, 42, 22], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="35" spans="1:11">
@@ -1787,10 +1820,10 @@
         <v>0</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>1</v>
+        <v>56</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>36</v>
@@ -1800,7 +1833,7 @@
       </c>
       <c r="K35" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.3, Y:0.6, Width: 0.05, Height: 0.1, Label: 33, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [32, 34, 43, 23], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.3, Y:0.6, Width: 0.05, Height: 0.1, Label: 33, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [32, 34, 43, 23], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="36" spans="1:11">
@@ -1823,10 +1856,10 @@
         <v>0</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>37</v>
@@ -1836,7 +1869,7 @@
       </c>
       <c r="K36" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.4, Y:0.6, Width: 0.05, Height: 0.1, Label: 34, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [33, 35, 44, 24], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.4, Y:0.6, Width: 0.05, Height: 0.1, Label: 34, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [33, 35, 44, 24], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="37" spans="1:11">
@@ -1856,13 +1889,13 @@
         <v>35</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>38</v>
@@ -1872,7 +1905,7 @@
       </c>
       <c r="K37" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.5, Y:0.6, Width: 0.05, Height: 0.1, Label: 35, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [34, 36, 45, 25], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.5, Y:0.6, Width: 0.05, Height: 0.1, Label: 35, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [34, 36, 45, 25], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="38" spans="1:11">
@@ -1892,13 +1925,13 @@
         <v>36</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I38" s="1" t="s">
         <v>39</v>
@@ -1908,7 +1941,7 @@
       </c>
       <c r="K38" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.6, Y:0.6, Width: 0.05, Height: 0.1, Label: 36, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [35, 37, 46, 26], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.6, Y:0.6, Width: 0.05, Height: 0.1, Label: 36, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [35, 37, 46, 26], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="39" spans="1:11">
@@ -1928,13 +1961,13 @@
         <v>37</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I39" s="1" t="s">
         <v>40</v>
@@ -1944,7 +1977,7 @@
       </c>
       <c r="K39" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.7, Y:0.6, Width: 0.05, Height: 0.1, Label: 37, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [36, 38, 47, 27], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.7, Y:0.6, Width: 0.05, Height: 0.1, Label: 37, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [36, 38, 47, 27], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="40" spans="1:11">
@@ -1964,13 +1997,13 @@
         <v>38</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>41</v>
@@ -1980,7 +2013,7 @@
       </c>
       <c r="K40" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.8, Y:0.6, Width: 0.05, Height: 0.1, Label: 38, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [37, 39, 48, 28], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.8, Y:0.6, Width: 0.05, Height: 0.1, Label: 38, acceptsArmy: false, acceptsFleet: true, isSupplyCenter: false, Connections: [37, 39, 48, 28], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="41" spans="1:11">
@@ -2003,10 +2036,10 @@
         <v>0</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>1</v>
+        <v>54</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I41" s="1" t="s">
         <v>42</v>
@@ -2016,7 +2049,7 @@
       </c>
       <c r="K41" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.9, Y:0.6, Width: 0.05, Height: 0.1, Label: 39, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [38,     49, 29], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.9, Y:0.6, Width: 0.05, Height: 0.1, Label: 39, acceptsArmy: true, acceptsFleet: true, isSupplyCenter: false, Connections: [38,     49, 29], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="42" spans="1:11">
@@ -2042,7 +2075,7 @@
         <v>1</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I42" s="1" t="s">
         <v>43</v>
@@ -2078,7 +2111,7 @@
         <v>1</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>44</v>
@@ -2088,7 +2121,7 @@
       </c>
       <c r="K43" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.1, Y:0.8, Width: 0.05, Height: 0.1, Label: 41, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [40, 42, 31], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.1, Y:0.8, Width: 0.05, Height: 0.1, Label: 41, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [40, 42, 31], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="44" spans="1:11">
@@ -2114,7 +2147,7 @@
         <v>1</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I44" s="1" t="s">
         <v>45</v>
@@ -2150,7 +2183,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I45" s="1" t="s">
         <v>46</v>
@@ -2160,7 +2193,7 @@
       </c>
       <c r="K45" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.3, Y:0.8, Width: 0.05, Height: 0.1, Label: 43, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [42, 44, 33], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.3, Y:0.8, Width: 0.05, Height: 0.1, Label: 43, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [42, 44, 33], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="46" spans="1:11">
@@ -2186,7 +2219,7 @@
         <v>1</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I46" s="1" t="s">
         <v>47</v>
@@ -2196,7 +2229,7 @@
       </c>
       <c r="K46" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.4, Y:0.8, Width: 0.05, Height: 0.1, Label: 44, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [43, 45, 34], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.4, Y:0.8, Width: 0.05, Height: 0.1, Label: 44, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [43, 45, 34], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="47" spans="1:11">
@@ -2216,13 +2249,13 @@
         <v>45</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G47" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I47" s="1" t="s">
         <v>48</v>
@@ -2232,7 +2265,7 @@
       </c>
       <c r="K47" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.5, Y:0.8, Width: 0.05, Height: 0.1, Label: 45, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [44, 46, 35], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.5, Y:0.8, Width: 0.05, Height: 0.1, Label: 45, acceptsArmy: false, acceptsFleet: false, isSupplyCenter: false, Connections: [44, 46, 35], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="48" spans="1:11">
@@ -2258,7 +2291,7 @@
         <v>1</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>0</v>
+        <v>54</v>
       </c>
       <c r="I48" s="1" t="s">
         <v>49</v>
@@ -2294,7 +2327,7 @@
         <v>1</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I49" s="1" t="s">
         <v>50</v>
@@ -2304,7 +2337,7 @@
       </c>
       <c r="K49" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.7, Y:0.8, Width: 0.05, Height: 0.1, Label: 47, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [46, 48, 37], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.7, Y:0.8, Width: 0.05, Height: 0.1, Label: 47, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [46, 48, 37], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -2324,13 +2357,13 @@
         <v>48</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>51</v>
@@ -2340,7 +2373,7 @@
       </c>
       <c r="K50" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.8, Y:0.8, Width: 0.05, Height: 0.1, Label: 48, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [47, 49, 38], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.8, Y:0.8, Width: 0.05, Height: 0.1, Label: 48, acceptsArmy: false, acceptsFleet: false, isSupplyCenter: false, Connections: [47, 49, 38], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -2366,7 +2399,7 @@
         <v>1</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="I51" s="1" t="s">
         <v>52</v>
@@ -2376,7 +2409,7 @@
       </c>
       <c r="K51" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>{ X: 0.9, Y:0.8, Width: 0.05, Height: 0.1, Label: 49, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: true, Connections: [48,     39], CostalRestrictions: [[]] }</v>
+        <v>{ X: 0.9, Y:0.8, Width: 0.05, Height: 0.1, Label: 49, acceptsArmy: true, acceptsFleet: false, isSupplyCenter: false, Connections: [48,     39], CostalRestrictions: [[]] }</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -2443,31 +2476,46 @@
       <c r="A63" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>